<commit_message>
Con lectura de coordinación
Para ajustes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCMarquez\Desktop\Versiones\CienciasSociales\fuentes\contenidos\grado07\guion02\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14520" tabRatio="729" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,16 +18,207 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>MCMarquez</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cambiar por el que puse en la caja inicial del manuscrito</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>MCMarquez</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+este corresponde a sección 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+arreglar</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+arreglar
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Falta incluir texto
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F107" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ajustar
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F124" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>MCMarquez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+completar</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,7 +612,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +690,19 @@
       <i/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2044,27 +2253,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -2072,7 +2281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -2080,7 +2289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="56">
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -2088,7 +2297,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -2096,7 +2305,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -2104,7 +2313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -2114,6 +2323,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2126,25 +2336,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2164,7 +2374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2184,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2224,7 +2434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2244,7 +2454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2264,7 +2474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2285,7 +2495,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2516,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2327,7 +2537,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2347,7 +2557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2367,7 +2577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2387,7 +2597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2407,7 +2617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2427,7 +2637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2447,7 +2657,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2467,7 +2677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2487,7 +2697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2507,7 +2717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2527,7 +2737,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2547,7 +2757,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2567,7 +2777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2587,7 +2797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2607,7 +2817,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2627,7 +2837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2647,7 +2857,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -2667,7 +2877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -2687,7 +2897,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -2707,7 +2917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2937,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2747,7 +2957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2767,7 +2977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -2787,7 +2997,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -2807,7 +3017,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -2845,14 +3055,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2863,7 +3073,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2874,7 +3084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="90">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>122</v>
       </c>
@@ -2885,12 +3095,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -2910,24 +3120,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2938,7 +3148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2949,7 +3159,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2960,7 +3170,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2971,7 +3181,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2982,7 +3192,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2993,7 +3203,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3004,7 +3214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3015,7 +3225,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3026,7 +3236,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="4" customFormat="1">
+    <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3037,7 +3247,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3048,7 +3258,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3059,7 +3269,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3070,7 +3280,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3081,7 +3291,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3092,7 +3302,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3103,7 +3313,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3114,7 +3324,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3125,7 +3335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3136,7 +3346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3147,7 +3357,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3158,7 +3368,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3169,7 +3379,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3180,7 +3390,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3191,7 +3401,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3202,7 +3412,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3213,7 +3423,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3224,7 +3434,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3235,7 +3445,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3246,7 +3456,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3257,7 +3467,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3268,7 +3478,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3279,7 +3489,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3290,7 +3500,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3301,7 +3511,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3312,7 +3522,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="42">
+    <row r="36" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3338,28 +3548,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="21" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>6</v>
       </c>
@@ -3388,7 +3598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
@@ -3403,7 +3613,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>23</v>
       </c>
@@ -3420,7 +3630,7 @@
       <c r="H3" s="19"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>23</v>
       </c>
@@ -3439,7 +3649,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>23</v>
       </c>
@@ -3456,7 +3666,7 @@
       <c r="H5" s="19"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" ht="28">
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>23</v>
       </c>
@@ -3473,7 +3683,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" ht="15">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>23</v>
       </c>
@@ -3488,7 +3698,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" ht="30">
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>23</v>
       </c>
@@ -3507,7 +3717,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>23</v>
       </c>
@@ -3526,7 +3736,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>23</v>
       </c>
@@ -3541,7 +3751,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" ht="15">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>23</v>
       </c>
@@ -3556,7 +3766,7 @@
       <c r="H11" s="19"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" ht="30">
+    <row r="12" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>23</v>
       </c>
@@ -3575,7 +3785,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>23</v>
       </c>
@@ -3590,7 +3800,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" ht="45">
+    <row r="14" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>23</v>
       </c>
@@ -3609,7 +3819,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>23</v>
       </c>
@@ -3624,7 +3834,7 @@
       <c r="H15" s="19"/>
       <c r="I15" s="18"/>
     </row>
-    <row r="16" spans="1:9" ht="30">
+    <row r="16" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
@@ -3643,7 +3853,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="42">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>23</v>
       </c>
@@ -3660,7 +3870,7 @@
       <c r="H17" s="19"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>23</v>
       </c>
@@ -3677,7 +3887,7 @@
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>23</v>
       </c>
@@ -3692,7 +3902,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>23</v>
       </c>
@@ -3707,7 +3917,7 @@
       <c r="H20" s="19"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" ht="45">
+    <row r="21" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>23</v>
       </c>
@@ -3726,7 +3936,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="45">
+    <row r="22" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>23</v>
       </c>
@@ -3745,7 +3955,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15">
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>23</v>
       </c>
@@ -3762,7 +3972,7 @@
       <c r="H23" s="19"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" ht="30">
+    <row r="24" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>23</v>
       </c>
@@ -3781,7 +3991,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30">
+    <row r="25" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="20" t="s">
         <v>81</v>
@@ -3796,7 +4006,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" ht="60">
+    <row r="26" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
@@ -3811,7 +4021,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -3824,7 +4034,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:9" ht="45">
+    <row r="28" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="21"/>
       <c r="C28" s="21"/>
@@ -3841,7 +4051,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -3856,7 +4066,7 @@
       <c r="H29" s="22"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -3871,7 +4081,7 @@
       <c r="H30" s="22"/>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -3884,7 +4094,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="21"/>
@@ -3897,7 +4107,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" ht="45">
+    <row r="33" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
@@ -3914,7 +4124,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="21"/>
       <c r="C34" s="21"/>
@@ -3927,7 +4137,7 @@
       <c r="H34" s="22"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -3940,7 +4150,7 @@
       <c r="H35" s="22"/>
       <c r="I35" s="18"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -3953,7 +4163,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
@@ -3966,7 +4176,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="21"/>
       <c r="C38" s="21"/>
@@ -3979,7 +4189,7 @@
       <c r="H38" s="22"/>
       <c r="I38" s="18"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="21"/>
       <c r="C39" s="21"/>
@@ -3992,7 +4202,7 @@
       <c r="H39" s="22"/>
       <c r="I39" s="18"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
@@ -4007,7 +4217,7 @@
       <c r="H40" s="22"/>
       <c r="I40" s="18"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -4020,7 +4230,7 @@
       <c r="H41" s="22"/>
       <c r="I41" s="18"/>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="21"/>
       <c r="C42" s="21"/>
@@ -4033,7 +4243,7 @@
       <c r="H42" s="22"/>
       <c r="I42" s="18"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="21"/>
       <c r="C43" s="21"/>
@@ -4046,7 +4256,7 @@
       <c r="H43" s="22"/>
       <c r="I43" s="18"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="21"/>
       <c r="C44" s="21"/>
@@ -4059,7 +4269,7 @@
       <c r="H44" s="22"/>
       <c r="I44" s="18"/>
     </row>
-    <row r="45" spans="1:9" ht="15">
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="21"/>
       <c r="C45" s="21"/>
@@ -4076,7 +4286,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15">
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="21"/>
       <c r="C46" s="21"/>
@@ -4091,7 +4301,7 @@
       <c r="H46" s="22"/>
       <c r="I46" s="18"/>
     </row>
-    <row r="47" spans="1:9" ht="45">
+    <row r="47" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
@@ -4108,7 +4318,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30">
+    <row r="48" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="21"/>
       <c r="C48" s="21"/>
@@ -4125,7 +4335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="14" t="s">
         <v>90</v>
@@ -4142,7 +4352,7 @@
       <c r="H49" s="22"/>
       <c r="I49" s="18"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
@@ -4155,7 +4365,7 @@
       <c r="H50" s="22"/>
       <c r="I50" s="18"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="21"/>
       <c r="C51" s="21"/>
@@ -4168,7 +4378,7 @@
       <c r="H51" s="22"/>
       <c r="I51" s="18"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
@@ -4181,7 +4391,7 @@
       <c r="H52" s="22"/>
       <c r="I52" s="18"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
@@ -4194,7 +4404,7 @@
       <c r="H53" s="22"/>
       <c r="I53" s="18"/>
     </row>
-    <row r="54" spans="1:9" ht="28">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
@@ -4211,7 +4421,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
@@ -4228,7 +4438,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
@@ -4243,7 +4453,7 @@
       <c r="H56" s="22"/>
       <c r="I56" s="18"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
@@ -4256,7 +4466,7 @@
       <c r="H57" s="22"/>
       <c r="I57" s="18"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="21"/>
       <c r="C58" s="21"/>
@@ -4269,7 +4479,7 @@
       <c r="H58" s="22"/>
       <c r="I58" s="18"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="21"/>
       <c r="C59" s="21"/>
@@ -4282,7 +4492,7 @@
       <c r="H59" s="22"/>
       <c r="I59" s="18"/>
     </row>
-    <row r="60" spans="1:9" ht="30">
+    <row r="60" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="21"/>
       <c r="C60" s="21"/>
@@ -4299,7 +4509,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="60">
+    <row r="61" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="21"/>
       <c r="C61" s="21"/>
@@ -4318,7 +4528,7 @@
       <c r="H61" s="22"/>
       <c r="I61" s="18"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="21"/>
       <c r="C62" s="21"/>
@@ -4331,7 +4541,7 @@
       <c r="H62" s="22"/>
       <c r="I62" s="18"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="21"/>
       <c r="C63" s="21"/>
@@ -4344,7 +4554,7 @@
       <c r="H63" s="22"/>
       <c r="I63" s="18"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="21"/>
       <c r="C64" s="21"/>
@@ -4357,7 +4567,7 @@
       <c r="H64" s="22"/>
       <c r="I64" s="18"/>
     </row>
-    <row r="65" spans="1:9" ht="45">
+    <row r="65" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A65" s="21"/>
       <c r="B65" s="21"/>
       <c r="C65" s="21"/>
@@ -4374,7 +4584,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="28">
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
       <c r="B66" s="21"/>
       <c r="C66" s="21"/>
@@ -4389,7 +4599,7 @@
       <c r="H66" s="22"/>
       <c r="I66" s="18"/>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
       <c r="B67" s="21"/>
       <c r="C67" s="21"/>
@@ -4404,7 +4614,7 @@
       <c r="H67" s="22"/>
       <c r="I67" s="18"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="21"/>
       <c r="B68" s="21"/>
       <c r="C68" s="21"/>
@@ -4417,7 +4627,7 @@
       <c r="H68" s="22"/>
       <c r="I68" s="18"/>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="21"/>
       <c r="C69" s="21"/>
@@ -4430,7 +4640,7 @@
       <c r="H69" s="22"/>
       <c r="I69" s="18"/>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="21"/>
       <c r="C70" s="21"/>
@@ -4445,7 +4655,7 @@
       <c r="H70" s="22"/>
       <c r="I70" s="18"/>
     </row>
-    <row r="71" spans="1:9" ht="45">
+    <row r="71" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="21"/>
       <c r="C71" s="21"/>
@@ -4460,7 +4670,7 @@
       <c r="H71" s="22"/>
       <c r="I71" s="18"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="21"/>
       <c r="C72" s="21"/>
@@ -4473,7 +4683,7 @@
       <c r="H72" s="22"/>
       <c r="I72" s="18"/>
     </row>
-    <row r="73" spans="1:9" ht="15">
+    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
       <c r="B73" s="21"/>
       <c r="C73" s="21"/>
@@ -4490,7 +4700,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30">
+    <row r="74" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
@@ -4507,7 +4717,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
       <c r="B75" s="21"/>
       <c r="C75" s="21"/>
@@ -4522,7 +4732,7 @@
       <c r="H75" s="22"/>
       <c r="I75" s="18"/>
     </row>
-    <row r="76" spans="1:9" ht="42">
+    <row r="76" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="21"/>
       <c r="C76" s="21"/>
@@ -4537,7 +4747,7 @@
       <c r="H76" s="22"/>
       <c r="I76" s="18"/>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="21"/>
       <c r="B77" s="21"/>
       <c r="C77" s="21"/>
@@ -4550,7 +4760,7 @@
       <c r="H77" s="22"/>
       <c r="I77" s="18"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="21"/>
       <c r="B78" s="21"/>
       <c r="C78" s="21"/>
@@ -4563,7 +4773,7 @@
       <c r="H78" s="22"/>
       <c r="I78" s="18"/>
     </row>
-    <row r="79" spans="1:9">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="21"/>
       <c r="C79" s="21"/>
@@ -4576,7 +4786,7 @@
       <c r="H79" s="22"/>
       <c r="I79" s="18"/>
     </row>
-    <row r="80" spans="1:9">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
       <c r="B80" s="21"/>
       <c r="C80" s="21"/>
@@ -4589,7 +4799,7 @@
       <c r="H80" s="22"/>
       <c r="I80" s="18"/>
     </row>
-    <row r="81" spans="1:9" ht="45">
+    <row r="81" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="21"/>
       <c r="C81" s="21"/>
@@ -4604,7 +4814,7 @@
       <c r="H81" s="22"/>
       <c r="I81" s="18"/>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
       <c r="B82" s="21"/>
       <c r="C82" s="21"/>
@@ -4617,7 +4827,7 @@
       <c r="H82" s="22"/>
       <c r="I82" s="18"/>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
@@ -4634,7 +4844,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A84" s="21"/>
       <c r="B84" s="21"/>
       <c r="C84" s="21"/>
@@ -4649,7 +4859,7 @@
       <c r="H84" s="22"/>
       <c r="I84" s="18"/>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
       <c r="B85" s="21"/>
       <c r="C85" s="21"/>
@@ -4662,7 +4872,7 @@
       <c r="H85" s="22"/>
       <c r="I85" s="18"/>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="21"/>
       <c r="B86" s="21"/>
       <c r="C86" s="21"/>
@@ -4675,7 +4885,7 @@
       <c r="H86" s="22"/>
       <c r="I86" s="18"/>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="21"/>
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
@@ -4690,7 +4900,7 @@
       <c r="H87" s="22"/>
       <c r="I87" s="18"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="21"/>
       <c r="B88" s="21"/>
       <c r="C88" s="21"/>
@@ -4703,7 +4913,7 @@
       <c r="H88" s="22"/>
       <c r="I88" s="18"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A89" s="21"/>
       <c r="B89" s="21"/>
       <c r="C89" s="21"/>
@@ -4720,7 +4930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
       <c r="B90" s="21"/>
       <c r="C90" s="21"/>
@@ -4735,7 +4945,7 @@
       <c r="H90" s="22"/>
       <c r="I90" s="18"/>
     </row>
-    <row r="91" spans="1:9" ht="60">
+    <row r="91" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
       <c r="B91" s="21"/>
       <c r="C91" s="21"/>
@@ -4750,7 +4960,7 @@
       <c r="H91" s="22"/>
       <c r="I91" s="18"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
       <c r="B92" s="21"/>
       <c r="C92" s="21"/>
@@ -4763,7 +4973,7 @@
       <c r="H92" s="22"/>
       <c r="I92" s="18"/>
     </row>
-    <row r="93" spans="1:9" ht="15">
+    <row r="93" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="21"/>
       <c r="B93" s="21"/>
       <c r="C93" s="21"/>
@@ -4780,7 +4990,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A94" s="21"/>
       <c r="B94" s="21"/>
       <c r="C94" s="21"/>
@@ -4795,7 +5005,7 @@
       <c r="H94" s="22"/>
       <c r="I94" s="18"/>
     </row>
-    <row r="95" spans="1:9" ht="30">
+    <row r="95" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A95" s="21"/>
       <c r="B95" s="21"/>
       <c r="C95" s="21"/>
@@ -4810,7 +5020,7 @@
       <c r="H95" s="22"/>
       <c r="I95" s="18"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="21"/>
       <c r="B96" s="21"/>
       <c r="C96" s="21"/>
@@ -4825,7 +5035,7 @@
       <c r="H96" s="22"/>
       <c r="I96" s="18"/>
     </row>
-    <row r="97" spans="1:9" ht="45">
+    <row r="97" spans="1:9" ht="63" x14ac:dyDescent="0.25">
       <c r="A97" s="21"/>
       <c r="B97" s="21"/>
       <c r="C97" s="21"/>
@@ -4842,7 +5052,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="30">
+    <row r="98" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" s="21"/>
       <c r="B98" s="20" t="s">
         <v>111</v>
@@ -4857,7 +5067,7 @@
       <c r="H98" s="22"/>
       <c r="I98" s="18"/>
     </row>
-    <row r="99" spans="1:9" ht="45">
+    <row r="99" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A99" s="21"/>
       <c r="B99" s="21"/>
       <c r="C99" s="21"/>
@@ -4872,7 +5082,7 @@
       <c r="H99" s="22"/>
       <c r="I99" s="18"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="21"/>
       <c r="B100" s="21"/>
       <c r="C100" s="21"/>
@@ -4885,7 +5095,7 @@
       <c r="H100" s="22"/>
       <c r="I100" s="18"/>
     </row>
-    <row r="101" spans="1:9" ht="45">
+    <row r="101" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A101" s="21"/>
       <c r="B101" s="21"/>
       <c r="C101" s="21"/>
@@ -4900,7 +5110,7 @@
       <c r="H101" s="22"/>
       <c r="I101" s="18"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="21"/>
       <c r="B102" s="21"/>
       <c r="C102" s="21"/>
@@ -4913,7 +5123,7 @@
       <c r="H102" s="22"/>
       <c r="I102" s="18"/>
     </row>
-    <row r="103" spans="1:9" ht="45">
+    <row r="103" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A103" s="21"/>
       <c r="B103" s="21"/>
       <c r="C103" s="21"/>
@@ -4928,7 +5138,7 @@
       <c r="H103" s="22"/>
       <c r="I103" s="18"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="21"/>
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
@@ -4941,7 +5151,7 @@
       <c r="H104" s="22"/>
       <c r="I104" s="18"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A105" s="21"/>
       <c r="B105" s="21"/>
       <c r="C105" s="21"/>
@@ -4958,7 +5168,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="15">
+    <row r="106" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
       <c r="B106" s="21"/>
       <c r="C106" s="21"/>
@@ -4973,7 +5183,7 @@
       <c r="H106" s="22"/>
       <c r="I106" s="18"/>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
       <c r="B107" s="21"/>
       <c r="C107" s="21"/>
@@ -4988,7 +5198,7 @@
       <c r="H107" s="22"/>
       <c r="I107" s="18"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="21"/>
       <c r="B108" s="21"/>
       <c r="C108" s="21"/>
@@ -5001,7 +5211,7 @@
       <c r="H108" s="22"/>
       <c r="I108" s="18"/>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="21"/>
       <c r="B109" s="21"/>
       <c r="C109" s="21"/>
@@ -5014,7 +5224,7 @@
       <c r="H109" s="22"/>
       <c r="I109" s="18"/>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="21"/>
       <c r="B110" s="21"/>
       <c r="C110" s="21"/>
@@ -5027,7 +5237,7 @@
       <c r="H110" s="22"/>
       <c r="I110" s="18"/>
     </row>
-    <row r="111" spans="1:9" ht="15">
+    <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="21"/>
       <c r="B111" s="21"/>
       <c r="C111" s="21"/>
@@ -5044,7 +5254,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="45">
+    <row r="112" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A112" s="21"/>
       <c r="B112" s="21"/>
       <c r="C112" s="21"/>
@@ -5061,7 +5271,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15">
+    <row r="113" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="21"/>
       <c r="B113" s="21"/>
       <c r="C113" s="21"/>
@@ -5074,7 +5284,7 @@
       <c r="H113" s="22"/>
       <c r="I113" s="18"/>
     </row>
-    <row r="114" spans="1:9" ht="15">
+    <row r="114" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="21"/>
       <c r="B114" s="21"/>
       <c r="C114" s="21"/>
@@ -5087,7 +5297,7 @@
       <c r="H114" s="22"/>
       <c r="I114" s="18"/>
     </row>
-    <row r="115" spans="1:9" ht="15">
+    <row r="115" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="21"/>
       <c r="B115" s="21"/>
       <c r="C115" s="21"/>
@@ -5100,7 +5310,7 @@
       <c r="H115" s="22"/>
       <c r="I115" s="18"/>
     </row>
-    <row r="116" spans="1:9" ht="15">
+    <row r="116" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="21"/>
       <c r="B116" s="21"/>
       <c r="C116" s="21"/>
@@ -5117,7 +5327,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="15">
+    <row r="117" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="21"/>
       <c r="B117" s="21"/>
       <c r="C117" s="21"/>
@@ -5130,7 +5340,7 @@
       <c r="H117" s="22"/>
       <c r="I117" s="18"/>
     </row>
-    <row r="118" spans="1:9" ht="15">
+    <row r="118" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="21"/>
       <c r="B118" s="21"/>
       <c r="C118" s="21"/>
@@ -5143,7 +5353,7 @@
       <c r="H118" s="22"/>
       <c r="I118" s="18"/>
     </row>
-    <row r="119" spans="1:9" ht="15">
+    <row r="119" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="21"/>
       <c r="B119" s="21"/>
       <c r="C119" s="21"/>
@@ -5156,7 +5366,7 @@
       <c r="H119" s="22"/>
       <c r="I119" s="18"/>
     </row>
-    <row r="120" spans="1:9" ht="15">
+    <row r="120" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="21"/>
       <c r="B120" s="21"/>
       <c r="C120" s="21"/>
@@ -5169,7 +5379,7 @@
       <c r="H120" s="22"/>
       <c r="I120" s="18"/>
     </row>
-    <row r="121" spans="1:9" ht="15">
+    <row r="121" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="21"/>
       <c r="B121" s="21"/>
       <c r="C121" s="21"/>
@@ -5186,7 +5396,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="30">
+    <row r="122" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" s="21"/>
       <c r="B122" s="21"/>
       <c r="C122" s="21"/>
@@ -5203,7 +5413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="30">
+    <row r="123" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A123" s="21"/>
       <c r="B123" s="21"/>
       <c r="C123" s="21"/>
@@ -5220,7 +5430,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="21"/>
       <c r="B124" s="21"/>
       <c r="C124" s="21"/>
@@ -5235,7 +5445,7 @@
       <c r="H124" s="22"/>
       <c r="I124" s="18"/>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="21"/>
       <c r="B125" s="21"/>
       <c r="C125" s="21"/>
@@ -5248,7 +5458,7 @@
       <c r="H125" s="22"/>
       <c r="I125" s="18"/>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="21"/>
       <c r="B126" s="21"/>
       <c r="C126" s="21"/>
@@ -5261,7 +5471,7 @@
       <c r="H126" s="22"/>
       <c r="I126" s="18"/>
     </row>
-    <row r="127" spans="1:9" ht="45">
+    <row r="127" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A127" s="21"/>
       <c r="B127" s="21"/>
       <c r="C127" s="21"/>
@@ -5278,7 +5488,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="21"/>
       <c r="B128" s="21"/>
       <c r="C128" s="21"/>
@@ -5291,7 +5501,7 @@
       <c r="H128" s="22"/>
       <c r="I128" s="18"/>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="21"/>
       <c r="B129" s="21"/>
       <c r="C129" s="21"/>
@@ -5306,7 +5516,7 @@
       <c r="H129" s="22"/>
       <c r="I129" s="18"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A130" s="21"/>
       <c r="B130" s="21"/>
       <c r="C130" s="21"/>
@@ -5323,7 +5533,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="21"/>
       <c r="B131" s="21" t="s">
         <v>123</v>
@@ -5342,7 +5552,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="1:9" ht="75">
+    <row r="132" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A132" s="21"/>
       <c r="B132" s="21"/>
       <c r="C132" s="21" t="s">
@@ -5361,6 +5571,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
En proceso de ajustes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="22640" windowHeight="13920" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="960" yWindow="0" windowWidth="24380" windowHeight="13820" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -3351,8 +3351,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="681">
+  <cellStyleXfs count="683">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4091,7 +4093,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="681">
+  <cellStyles count="683">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -4432,6 +4434,7 @@
     <cellStyle name="Hipervínculo" xfId="675" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="677" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="681" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -4772,6 +4775,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="676" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="678" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="680" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="682" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5042,7 +5046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5125,7 +5129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -5848,7 +5852,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6360,7 +6363,6 @@
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -6373,9 +6375,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F126" sqref="F126:F135"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9234,7 +9236,7 @@
         <v>79</v>
       </c>
       <c r="E132" s="22" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F132" s="22" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Versión final con nueva enumeración
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="118">
   <si>
     <t>FICHA</t>
   </si>
@@ -450,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,12 +544,6 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
@@ -598,7 +592,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="687">
+  <cellStyleXfs count="753">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1286,8 +1280,74 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1348,11 +1408,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="687">
+  <cellStyles count="753">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1696,6 +1753,39 @@
     <cellStyle name="Hipervínculo" xfId="681" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="683" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="751" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -2039,6 +2129,39 @@
     <cellStyle name="Hipervínculo visitado" xfId="682" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="684" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="686" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="752" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2309,7 +2432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2379,7 +2502,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3639,9 +3761,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F106" sqref="F106:F131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3699,6 +3821,12 @@
       <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="15">
+      <c r="A3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D3" s="21" t="s">
         <v>108</v>
       </c>
@@ -3707,6 +3835,15 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15">
+      <c r="A4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>108</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>70</v>
       </c>
@@ -3718,6 +3855,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D5" s="21" t="s">
         <v>71</v>
       </c>
@@ -3726,6 +3869,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30">
+      <c r="A6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D6" s="21" t="s">
         <v>72</v>
       </c>
@@ -3733,12 +3882,30 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="30">
+      <c r="A7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30">
+      <c r="A8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>70</v>
       </c>
@@ -3750,6 +3917,15 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
+      <c r="A9" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>74</v>
       </c>
@@ -3760,17 +3936,44 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="30">
+      <c r="A10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E10" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="30">
+      <c r="A11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30">
+      <c r="A12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>70</v>
       </c>
@@ -3781,12 +3984,30 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="30">
+      <c r="A13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45">
+      <c r="A14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>74</v>
       </c>
@@ -3797,12 +4018,30 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="30">
+      <c r="A15" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E15" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30">
+      <c r="A16" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3813,7 +4052,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="4:9" ht="45">
+    <row r="17" spans="1:9" ht="45">
+      <c r="A17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D17" s="21" t="s">
         <v>77</v>
       </c>
@@ -3821,7 +4066,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="4:9" ht="15">
+    <row r="18" spans="1:9" ht="15">
+      <c r="A18" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D18" s="21" t="s">
         <v>78</v>
       </c>
@@ -3829,17 +4080,44 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="4:9">
+    <row r="19" spans="1:9" ht="15">
+      <c r="A19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E19" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="4:9">
+    <row r="20" spans="1:9" ht="15">
+      <c r="A20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E20" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="4:9" ht="45">
+    <row r="21" spans="1:9" ht="45">
+      <c r="A21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E21" s="3" t="s">
         <v>74</v>
       </c>
@@ -3850,7 +4128,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="4:9" ht="45">
+    <row r="22" spans="1:9" ht="45">
+      <c r="A22" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E22" s="3" t="s">
         <v>70</v>
       </c>
@@ -3861,7 +4148,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="4:9" ht="30">
+    <row r="23" spans="1:9" ht="30">
+      <c r="A23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E23" s="3" t="s">
         <v>74</v>
       </c>
@@ -3872,7 +4168,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="4:9" ht="60">
+    <row r="24" spans="1:9" ht="60">
+      <c r="A24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D24" s="23" t="s">
         <v>111</v>
       </c>
@@ -3880,7 +4182,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="4:9" ht="60">
+    <row r="25" spans="1:9" ht="60">
+      <c r="A25" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="F25" s="21" t="s">
         <v>81</v>
       </c>
@@ -3888,12 +4199,36 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="4:9">
+    <row r="26" spans="1:9" ht="60">
+      <c r="A26" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>81</v>
+      </c>
       <c r="G26" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="4:9" ht="45">
+    <row r="27" spans="1:9" ht="60">
+      <c r="A27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>81</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>70</v>
       </c>
@@ -3904,7 +4239,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="4:9" ht="15">
+    <row r="28" spans="1:9" ht="60">
+      <c r="A28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>111</v>
+      </c>
       <c r="F28" s="21" t="s">
         <v>106</v>
       </c>
@@ -3912,17 +4256,53 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="4:9">
+    <row r="29" spans="1:9" ht="60">
+      <c r="A29" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="4:9">
+    <row r="30" spans="1:9" ht="60">
+      <c r="A30" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G30" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="4:9" ht="45">
+    <row r="31" spans="1:9" ht="60">
+      <c r="A31" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G31" s="3" t="s">
         <v>74</v>
       </c>
@@ -3933,62 +4313,206 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="4:9">
+    <row r="32" spans="1:9" ht="60">
+      <c r="A32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G32" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="1:9" ht="60">
+      <c r="A33" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G33" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="1:9" ht="60">
+      <c r="A34" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G34" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="2:9">
+    <row r="35" spans="1:9" ht="60">
+      <c r="A35" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G35" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="2:9">
+    <row r="36" spans="1:9" ht="60">
+      <c r="A36" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G36" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="2:9">
+    <row r="37" spans="1:9" ht="60">
+      <c r="A37" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G37" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="2:9">
+    <row r="38" spans="1:9" ht="60">
+      <c r="A38" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G38" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="2:9">
+    <row r="39" spans="1:9" ht="60">
+      <c r="A39" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G39" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="2:9">
+    <row r="40" spans="1:9" ht="60">
+      <c r="A40" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G40" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="2:9">
+    <row r="41" spans="1:9" ht="60">
+      <c r="A41" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G41" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="2:9">
+    <row r="42" spans="1:9" ht="60">
+      <c r="A42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G42" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="2:9" ht="15">
+    <row r="43" spans="1:9" ht="60">
+      <c r="A43" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G43" s="3" t="s">
         <v>70</v>
       </c>
@@ -3999,18 +4523,39 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="15">
+    <row r="44" spans="1:9" ht="15">
+      <c r="A44" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>68</v>
+      </c>
       <c r="D44" s="21" t="s">
         <v>79</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="2:9" ht="45">
+      <c r="F44" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="45">
+      <c r="A45" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>79</v>
+      </c>
       <c r="E45" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F45" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H45" s="22" t="s">
         <v>82</v>
       </c>
@@ -4018,10 +4563,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="2:9" ht="30">
+    <row r="46" spans="1:9" ht="30">
+      <c r="A46" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>79</v>
+      </c>
       <c r="E46" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F46" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H46" s="22" t="s">
         <v>83</v>
       </c>
@@ -4029,46 +4586,124 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="2:9">
+    <row r="47" spans="1:9" ht="15">
+      <c r="A47" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="B47" s="24" t="s">
         <v>84</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="48" spans="2:9" ht="15">
+      <c r="D47" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15">
+      <c r="A48" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D48" s="21" t="s">
         <v>85</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="49" spans="4:9">
+      <c r="F48" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15">
+      <c r="A49" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E49" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="50" spans="4:9">
+      <c r="F49" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15">
+      <c r="A50" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E50" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="51" spans="4:9">
+      <c r="F50" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15">
+      <c r="A51" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E51" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="52" spans="4:9">
+      <c r="F51" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15">
+      <c r="A52" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E52" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="4:9" ht="30">
+      <c r="F52" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30">
+      <c r="A53" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E53" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="F53" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H53" s="22" t="s">
         <v>42</v>
       </c>
@@ -4076,10 +4711,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="4:9" ht="30">
+    <row r="54" spans="1:9" ht="30">
+      <c r="A54" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="21" t="s">
+        <v>85</v>
+      </c>
       <c r="E54" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F54" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H54" s="25" t="s">
         <v>43</v>
       </c>
@@ -4087,33 +4734,90 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="4:9" ht="30">
+    <row r="55" spans="1:9" ht="30">
+      <c r="A55" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D55" s="21" t="s">
         <v>86</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="4:9">
+      <c r="F55" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30">
+      <c r="A56" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="E56" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="57" spans="4:9">
+      <c r="F56" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30">
+      <c r="A57" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="E57" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="58" spans="4:9">
+      <c r="F57" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30">
+      <c r="A58" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="E58" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="59" spans="4:9" ht="30">
+      <c r="F58" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="30">
+      <c r="A59" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>86</v>
+      </c>
       <c r="E59" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="F59" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H59" s="22" t="s">
         <v>44</v>
       </c>
@@ -4121,15 +4825,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="4:9" ht="32">
-      <c r="D60" s="26" t="s">
+    <row r="60" spans="1:9" ht="15">
+      <c r="A60" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="21" t="s">
         <v>87</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="4:9" ht="60">
+      <c r="F60" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="60">
+      <c r="A61" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="F61" s="21" t="s">
         <v>88</v>
       </c>
@@ -4137,22 +4859,70 @@
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="4:9">
+    <row r="62" spans="1:9" ht="60">
+      <c r="A62" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G62" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="4:9">
+    <row r="63" spans="1:9" ht="60">
+      <c r="A63" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G63" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="4:9">
+    <row r="64" spans="1:9" ht="60">
+      <c r="A64" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G64" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="4:9" ht="45">
+    <row r="65" spans="1:9" ht="60">
+      <c r="A65" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F65" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="G65" s="3" t="s">
         <v>74</v>
       </c>
@@ -4163,7 +4933,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="4:9" ht="30">
+    <row r="66" spans="1:9" ht="30">
+      <c r="A66" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="F66" s="21" t="s">
         <v>89</v>
       </c>
@@ -4171,7 +4950,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="4:9" ht="30">
+    <row r="67" spans="1:9" ht="30">
+      <c r="A67" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="F67" s="21" t="s">
         <v>90</v>
       </c>
@@ -4179,17 +4967,50 @@
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="4:9">
+    <row r="68" spans="1:9" ht="30">
+      <c r="A68" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F68" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="G68" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="4:9">
+    <row r="69" spans="1:9" ht="30">
+      <c r="A69" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>90</v>
+      </c>
       <c r="G69" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="4:9" ht="30">
+    <row r="70" spans="1:9" ht="30">
+      <c r="A70" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="F70" s="21" t="s">
         <v>91</v>
       </c>
@@ -4197,7 +5018,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="4:9" ht="45">
+    <row r="71" spans="1:9" ht="45">
+      <c r="A71" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>87</v>
+      </c>
       <c r="F71" s="21" t="s">
         <v>92</v>
       </c>
@@ -4205,12 +5035,36 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="4:9">
+    <row r="72" spans="1:9" ht="45">
+      <c r="A72" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="G72" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="4:9" ht="15">
+    <row r="73" spans="1:9" ht="45">
+      <c r="A73" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F73" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="G73" s="3" t="s">
         <v>70</v>
       </c>
@@ -4221,7 +5075,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="4:9" ht="28">
+    <row r="74" spans="1:9" ht="45">
+      <c r="A74" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74" s="21" t="s">
+        <v>92</v>
+      </c>
       <c r="G74" s="3" t="s">
         <v>74</v>
       </c>
@@ -4232,15 +5098,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="4:9" ht="15">
+    <row r="75" spans="1:9" ht="45">
+      <c r="A75" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D75" s="21" t="s">
         <v>93</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="76" spans="4:9" ht="60">
+      <c r="F75" s="21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="60">
+      <c r="A76" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D76" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="F76" s="21" t="s">
         <v>94</v>
       </c>
@@ -4248,27 +5132,84 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="4:9">
+    <row r="77" spans="1:9" ht="60">
+      <c r="A77" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F77" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="G77" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="4:9">
+    <row r="78" spans="1:9" ht="60">
+      <c r="A78" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D78" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F78" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="G78" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="4:9">
+    <row r="79" spans="1:9" ht="60">
+      <c r="A79" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="G79" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="4:9">
+    <row r="80" spans="1:9" ht="60">
+      <c r="A80" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" s="21" t="s">
+        <v>94</v>
+      </c>
       <c r="G80" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="4:9" ht="45">
+    <row r="81" spans="1:9" ht="45">
+      <c r="A81" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="F81" s="21" t="s">
         <v>96</v>
       </c>
@@ -4276,12 +5217,36 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="4:9">
+    <row r="82" spans="1:9" ht="45">
+      <c r="A82" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" s="21" t="s">
+        <v>96</v>
+      </c>
       <c r="G82" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="4:9" ht="30">
+    <row r="83" spans="1:9" ht="45">
+      <c r="A83" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D83" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F83" s="21" t="s">
+        <v>96</v>
+      </c>
       <c r="G83" s="3" t="s">
         <v>70</v>
       </c>
@@ -4292,7 +5257,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="4:9" ht="30">
+    <row r="84" spans="1:9" ht="30">
+      <c r="A84" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D84" s="21" t="s">
+        <v>93</v>
+      </c>
       <c r="F84" s="21" t="s">
         <v>98</v>
       </c>
@@ -4300,33 +5274,90 @@
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="4:9">
+    <row r="85" spans="1:9" ht="30">
+      <c r="A85" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F85" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="G85" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="4:9">
+    <row r="86" spans="1:9" ht="30">
+      <c r="A86" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F86" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="G86" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="4:9" ht="15">
+    <row r="87" spans="1:9" ht="30">
+      <c r="A87" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D87" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="88" spans="4:9">
+      <c r="F87" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="30">
+      <c r="A88" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D88" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E88" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="89" spans="4:9" ht="45">
+      <c r="F88" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="45">
+      <c r="A89" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>78</v>
+      </c>
       <c r="E89" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F89" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="H89" s="22" t="s">
         <v>114</v>
       </c>
@@ -4334,15 +5365,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="4:9" ht="30">
+    <row r="90" spans="1:9" ht="30">
+      <c r="A90" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D90" s="21" t="s">
         <v>99</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="91" spans="4:9" ht="60">
+      <c r="F90" s="21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="60">
+      <c r="A91" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="F91" s="21" t="s">
         <v>100</v>
       </c>
@@ -4350,12 +5399,36 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="4:9">
+    <row r="92" spans="1:9" ht="60">
+      <c r="A92" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F92" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="G92" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="4:9">
+    <row r="93" spans="1:9" ht="60">
+      <c r="A93" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D93" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F93" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="G93" s="3" t="s">
         <v>70</v>
       </c>
@@ -4366,7 +5439,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="4:9" ht="30">
+    <row r="94" spans="1:9" ht="30">
+      <c r="A94" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="F94" s="21" t="s">
         <v>101</v>
       </c>
@@ -4374,7 +5456,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="4:9" ht="30">
+    <row r="95" spans="1:9" ht="30">
+      <c r="A95" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>99</v>
+      </c>
       <c r="F95" s="21" t="s">
         <v>102</v>
       </c>
@@ -4382,7 +5473,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="4:9" ht="45">
+    <row r="96" spans="1:9" ht="45">
+      <c r="A96" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D96" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F96" s="21" t="s">
+        <v>102</v>
+      </c>
       <c r="G96" s="3" t="s">
         <v>74</v>
       </c>
@@ -4393,15 +5496,33 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="4:9" ht="60">
+    <row r="97" spans="1:9" ht="60">
+      <c r="A97" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D97" s="21" t="s">
         <v>115</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="98" spans="4:9" ht="45">
+      <c r="F97" s="21" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="60">
+      <c r="A98" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D98" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="F98" s="21" t="s">
         <v>104</v>
       </c>
@@ -4409,12 +5530,33 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="4:9">
+    <row r="99" spans="1:9" ht="60">
+      <c r="A99" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D99" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F99" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="G99" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="100" spans="4:9" ht="45">
+    <row r="100" spans="1:9" ht="60">
+      <c r="A100" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D100" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="F100" s="21" t="s">
         <v>105</v>
       </c>
@@ -4422,12 +5564,33 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="4:9">
+    <row r="101" spans="1:9" ht="60">
+      <c r="A101" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D101" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F101" s="21" t="s">
+        <v>105</v>
+      </c>
       <c r="G101" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="102" spans="4:9" ht="45">
+    <row r="102" spans="1:9" ht="60">
+      <c r="A102" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B102" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D102" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="F102" s="21" t="s">
         <v>52</v>
       </c>
@@ -4435,12 +5598,36 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="4:9">
+    <row r="103" spans="1:9" ht="60">
+      <c r="A103" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D103" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F103" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="G103" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="104" spans="4:9" ht="30">
+    <row r="104" spans="1:9" ht="60">
+      <c r="A104" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D104" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F104" s="21" t="s">
+        <v>52</v>
+      </c>
       <c r="G104" s="3" t="s">
         <v>70</v>
       </c>
@@ -4451,7 +5638,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="4:9" ht="15">
+    <row r="105" spans="1:9" ht="60">
+      <c r="A105" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D105" s="21" t="s">
+        <v>115</v>
+      </c>
       <c r="F105" s="21" t="s">
         <v>106</v>
       </c>
@@ -4459,22 +5655,70 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="4:9">
+    <row r="106" spans="1:9" ht="60">
+      <c r="A106" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D106" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F106" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G106" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="4:9">
+    <row r="107" spans="1:9" ht="60">
+      <c r="A107" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D107" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G107" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="4:9">
+    <row r="108" spans="1:9" ht="60">
+      <c r="A108" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D108" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F108" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G108" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="4:9" ht="15">
+    <row r="109" spans="1:9" ht="60">
+      <c r="A109" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D109" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F109" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G109" s="3" t="s">
         <v>70</v>
       </c>
@@ -4485,7 +5729,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="110" spans="4:9" ht="45">
+    <row r="110" spans="1:9" ht="60">
+      <c r="A110" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B110" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D110" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F110" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G110" s="3" t="s">
         <v>74</v>
       </c>
@@ -4496,22 +5752,70 @@
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="4:9">
+    <row r="111" spans="1:9" ht="60">
+      <c r="A111" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D111" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F111" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G111" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="4:9">
+    <row r="112" spans="1:9" ht="60">
+      <c r="A112" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D112" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F112" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G112" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="113" spans="4:9">
+    <row r="113" spans="1:9" ht="60">
+      <c r="A113" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D113" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F113" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G113" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="4:9">
+    <row r="114" spans="1:9" ht="60">
+      <c r="A114" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D114" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F114" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G114" s="3" t="s">
         <v>70</v>
       </c>
@@ -4522,27 +5826,87 @@
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="4:9">
+    <row r="115" spans="1:9" ht="60">
+      <c r="A115" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D115" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F115" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G115" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="4:9">
+    <row r="116" spans="1:9" ht="60">
+      <c r="A116" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D116" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F116" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G116" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="4:9">
+    <row r="117" spans="1:9" ht="60">
+      <c r="A117" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F117" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G117" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="4:9">
+    <row r="118" spans="1:9" ht="60">
+      <c r="A118" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D118" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F118" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G118" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="4:9">
+    <row r="119" spans="1:9" ht="60">
+      <c r="A119" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D119" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F119" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G119" s="3" t="s">
         <v>70</v>
       </c>
@@ -4553,7 +5917,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="120" spans="4:9" ht="30">
+    <row r="120" spans="1:9" ht="60">
+      <c r="A120" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D120" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F120" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G120" s="3" t="s">
         <v>70</v>
       </c>
@@ -4564,7 +5940,19 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="4:9" ht="28">
+    <row r="121" spans="1:9" ht="60">
+      <c r="A121" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D121" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F121" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G121" s="3" t="s">
         <v>74</v>
       </c>
@@ -4575,22 +5963,70 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="4:9">
+    <row r="122" spans="1:9" ht="60">
+      <c r="A122" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B122" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D122" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F122" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G122" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="4:9">
+    <row r="123" spans="1:9" ht="60">
+      <c r="A123" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B123" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D123" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F123" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G123" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="124" spans="4:9">
+    <row r="124" spans="1:9" ht="60">
+      <c r="A124" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B124" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D124" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F124" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G124" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="4:9" ht="28">
+    <row r="125" spans="1:9" ht="60">
+      <c r="A125" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B125" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D125" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F125" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G125" s="3" t="s">
         <v>74</v>
       </c>
@@ -4601,23 +6037,56 @@
         <v>66</v>
       </c>
     </row>
-    <row r="126" spans="4:9">
+    <row r="126" spans="1:9" ht="60">
+      <c r="A126" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B126" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D126" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F126" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="G126" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="4:9" ht="15">
+    <row r="127" spans="1:9" ht="15">
+      <c r="A127" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B127" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="D127" s="20" t="s">
         <v>79</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="128" spans="4:9" ht="30">
+      <c r="F127" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="30">
+      <c r="A128" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B128" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D128" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="E128" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F128" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H128" s="22" t="s">
         <v>107</v>
       </c>
@@ -4625,10 +6094,22 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" spans="2:9" ht="30">
+    <row r="129" spans="1:9" ht="30">
+      <c r="A129" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B129" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D129" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="E129" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="F129" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="H129" s="22" t="s">
         <v>113</v>
       </c>
@@ -4636,17 +6117,38 @@
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="2:9" ht="15">
+    <row r="130" spans="1:9" ht="15">
+      <c r="A130" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="B130" s="20" t="s">
         <v>110</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="131" spans="2:9" ht="70">
+      <c r="D130" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F130" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="70">
+      <c r="A131" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131" s="20" t="s">
+        <v>110</v>
+      </c>
       <c r="C131" s="3" t="s">
         <v>117</v>
+      </c>
+      <c r="D131" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F131" s="21" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versión final con los ajustes indicados por Oliver C.
Nota: No se encontró una coincidencia el título del recurso Refuerza tu
aprendizaje: La Iglesia en la baja edad media no se encontró en el
listado de aula planeta. Se unificó como aparecía en el recurso
aprovechado tomado de aulaplaneta y se modificó en el cuaderno de
estudio.

Eugeniarce
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="107">
   <si>
     <t>FICHA</t>
   </si>
@@ -287,12 +287,6 @@
     <t>Practica</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: la nobleza</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: los campesinos</t>
-  </si>
-  <si>
     <t>La economía de subsistencia</t>
   </si>
   <si>
@@ -308,12 +302,6 @@
     <t>Los monasterios y las órdenes religiosas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el arte y la cultura bizantinos</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: el arte mozárabe</t>
-  </si>
-  <si>
     <t xml:space="preserve">La Baja Edad Media </t>
   </si>
   <si>
@@ -353,9 +341,6 @@
     <t>Los nuevos espacios urbanos</t>
   </si>
   <si>
-    <t>El nuevo paisaje urbano en la Baja Edad Media</t>
-  </si>
-  <si>
     <t>El gobierno de las ciudades</t>
   </si>
   <si>
@@ -371,9 +356,6 @@
     <t>Las revueltas urbanas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La crisis de la Baja Edad Media</t>
-  </si>
-  <si>
     <t>El pensamiento medieval</t>
   </si>
   <si>
@@ -383,17 +365,9 @@
     <t xml:space="preserve">El arte </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: el arte gótico</t>
-  </si>
-  <si>
     <t>El feudo</t>
   </si>
   <si>
-    <t xml:space="preserve">Autoevaluación
-Evalúa tus conocimientos sobre el tema del feudalismo
-</t>
-  </si>
-  <si>
     <t>Fin de tema</t>
   </si>
   <si>
@@ -406,51 +380,14 @@
     <t>Refuerza tu aprendizaje: El arte mudéjar</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: La Iglesia en la baja edad media</t>
-  </si>
-  <si>
     <t>La cultura y el arte de la Baja Edad Media</t>
-  </si>
-  <si>
-    <r>
-      <t>Analizar un cuadro</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>La</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> Piedad de Avignon</t>
-    </r>
-  </si>
-  <si>
-    <t>Autoevaluación Evalúa tus conocimientos sobre el tema del feudalismo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -543,12 +480,6 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -592,8 +523,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="761">
+  <cellStyleXfs count="783">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1417,7 +1370,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="761">
+  <cellStyles count="783">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1798,6 +1751,17 @@
     <cellStyle name="Hipervínculo" xfId="755" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="757" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="781" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -2178,6 +2142,17 @@
     <cellStyle name="Hipervínculo visitado" xfId="756" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="758" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="776" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="778" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="780" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="782" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2489,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2531,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3243,7 +3218,7 @@
         <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E35" t="s">
         <v>53</v>
@@ -3254,6 +3229,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3267,7 +3243,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3299,9 +3275,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="90">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="15">
       <c r="A3" s="17" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
@@ -3340,8 +3316,8 @@
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3731,7 +3707,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>66</v>
@@ -3748,12 +3724,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="42">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>64</v>
@@ -3778,8 +3754,8 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3844,7 +3820,7 @@
         <v>68</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>69</v>
@@ -3858,7 +3834,7 @@
         <v>68</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>70</v>
@@ -3945,8 +3921,8 @@
       <c r="E9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H9" s="22" t="s">
-        <v>75</v>
+      <c r="H9" t="s">
+        <v>29</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>66</v>
@@ -4061,8 +4037,8 @@
       <c r="E16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="22" t="s">
-        <v>76</v>
+      <c r="H16" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>66</v>
@@ -4076,7 +4052,7 @@
         <v>68</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>69</v>
@@ -4090,7 +4066,7 @@
         <v>68</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>69</v>
@@ -4104,7 +4080,7 @@
         <v>68</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>73</v>
@@ -4118,7 +4094,7 @@
         <v>68</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>69</v>
@@ -4132,7 +4108,7 @@
         <v>68</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>74</v>
@@ -4152,7 +4128,7 @@
         <v>68</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>70</v>
@@ -4172,13 +4148,13 @@
         <v>68</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>74</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>66</v>
@@ -4192,7 +4168,7 @@
         <v>68</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>69</v>
@@ -4206,10 +4182,10 @@
         <v>68</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>69</v>
@@ -4223,10 +4199,10 @@
         <v>68</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>73</v>
@@ -4240,10 +4216,10 @@
         <v>68</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>70</v>
@@ -4263,10 +4239,10 @@
         <v>68</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>69</v>
@@ -4280,10 +4256,10 @@
         <v>68</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>73</v>
@@ -4297,13 +4273,13 @@
         <v>68</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45">
@@ -4314,10 +4290,10 @@
         <v>68</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>74</v>
@@ -4337,10 +4313,10 @@
         <v>68</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>69</v>
@@ -4354,10 +4330,10 @@
         <v>68</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>73</v>
@@ -4371,10 +4347,10 @@
         <v>68</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>69</v>
@@ -4388,10 +4364,10 @@
         <v>68</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>73</v>
@@ -4405,10 +4381,10 @@
         <v>68</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>69</v>
@@ -4422,10 +4398,10 @@
         <v>68</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>73</v>
@@ -4439,10 +4415,10 @@
         <v>68</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>69</v>
@@ -4456,10 +4432,10 @@
         <v>68</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>73</v>
@@ -4473,10 +4449,10 @@
         <v>68</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>69</v>
@@ -4490,10 +4466,10 @@
         <v>68</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>73</v>
@@ -4507,13 +4483,13 @@
         <v>68</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="45">
@@ -4524,10 +4500,10 @@
         <v>68</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>70</v>
@@ -4547,16 +4523,16 @@
         <v>68</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28">
       <c r="A45" s="13" t="s">
         <v>23</v>
       </c>
@@ -4564,22 +4540,22 @@
         <v>68</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>82</v>
+        <v>100</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="I45" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9" ht="28">
       <c r="A46" s="13" t="s">
         <v>23</v>
       </c>
@@ -4587,16 +4563,16 @@
         <v>68</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>83</v>
+        <v>100</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>66</v>
@@ -4607,7 +4583,7 @@
         <v>23</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>69</v>
@@ -4618,10 +4594,10 @@
         <v>23</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>69</v>
@@ -4633,10 +4609,10 @@
         <v>23</v>
       </c>
       <c r="B49" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>73</v>
@@ -4648,10 +4624,10 @@
         <v>23</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>69</v>
@@ -4663,10 +4639,10 @@
         <v>23</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>73</v>
@@ -4678,10 +4654,10 @@
         <v>23</v>
       </c>
       <c r="B52" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D52" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>69</v>
@@ -4693,10 +4669,10 @@
         <v>23</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D53" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>70</v>
@@ -4714,10 +4690,10 @@
         <v>23</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D54" s="21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>74</v>
@@ -4735,10 +4711,10 @@
         <v>23</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>69</v>
@@ -4750,10 +4726,10 @@
         <v>23</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>73</v>
@@ -4765,10 +4741,10 @@
         <v>23</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>69</v>
@@ -4780,10 +4756,10 @@
         <v>23</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>73</v>
@@ -4795,10 +4771,10 @@
         <v>23</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>70</v>
@@ -4816,10 +4792,10 @@
         <v>23</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>69</v>
@@ -4831,13 +4807,13 @@
         <v>23</v>
       </c>
       <c r="B61" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F61" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>88</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>69</v>
@@ -4848,13 +4824,13 @@
         <v>23</v>
       </c>
       <c r="B62" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F62" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="D62" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>88</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>73</v>
@@ -4865,13 +4841,13 @@
         <v>23</v>
       </c>
       <c r="B63" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F63" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="D63" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>88</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>69</v>
@@ -4882,13 +4858,13 @@
         <v>23</v>
       </c>
       <c r="B64" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F64" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="D64" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F64" s="21" t="s">
-        <v>88</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>73</v>
@@ -4899,13 +4875,13 @@
         <v>23</v>
       </c>
       <c r="B65" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F65" s="21" t="s">
         <v>84</v>
-      </c>
-      <c r="D65" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>88</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>74</v>
@@ -4922,13 +4898,13 @@
         <v>23</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>69</v>
@@ -4939,13 +4915,13 @@
         <v>23</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>69</v>
@@ -4956,13 +4932,13 @@
         <v>23</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>73</v>
@@ -4973,13 +4949,13 @@
         <v>23</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>69</v>
@@ -4990,13 +4966,13 @@
         <v>23</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D70" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F70" s="21" t="s">
         <v>87</v>
-      </c>
-      <c r="F70" s="21" t="s">
-        <v>91</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>69</v>
@@ -5007,13 +4983,13 @@
         <v>23</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>69</v>
@@ -5024,13 +5000,13 @@
         <v>23</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>73</v>
@@ -5041,13 +5017,13 @@
         <v>23</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>70</v>
@@ -5064,13 +5040,13 @@
         <v>23</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>74</v>
@@ -5087,10 +5063,10 @@
         <v>23</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>69</v>
@@ -5102,13 +5078,13 @@
         <v>23</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>69</v>
@@ -5119,13 +5095,13 @@
         <v>23</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F77" s="21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>73</v>
@@ -5136,13 +5112,13 @@
         <v>23</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>69</v>
@@ -5153,13 +5129,13 @@
         <v>23</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F79" s="21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>73</v>
@@ -5170,16 +5146,16 @@
         <v>23</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="30">
@@ -5187,13 +5163,13 @@
         <v>23</v>
       </c>
       <c r="B81" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>69</v>
@@ -5204,13 +5180,13 @@
         <v>23</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>73</v>
@@ -5221,19 +5197,19 @@
         <v>23</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H83" s="22" t="s">
-        <v>97</v>
+      <c r="H83" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>66</v>
@@ -5244,13 +5220,13 @@
         <v>23</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D84" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F84" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="F84" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>69</v>
@@ -5261,13 +5237,13 @@
         <v>23</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D85" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="F85" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>73</v>
@@ -5278,13 +5254,13 @@
         <v>23</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D86" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F86" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="F86" s="21" t="s">
-        <v>98</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>69</v>
@@ -5295,10 +5271,10 @@
         <v>23</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D87" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>69</v>
@@ -5310,32 +5286,32 @@
         <v>23</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D88" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F88" s="21"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" ht="15">
       <c r="A89" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D89" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F89" s="21"/>
-      <c r="H89" s="22" t="s">
-        <v>114</v>
+      <c r="H89" t="s">
+        <v>48</v>
       </c>
       <c r="I89" s="5" t="s">
         <v>66</v>
@@ -5346,10 +5322,10 @@
         <v>23</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>69</v>
@@ -5361,13 +5337,13 @@
         <v>23</v>
       </c>
       <c r="B91" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D91" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>69</v>
@@ -5378,13 +5354,13 @@
         <v>23</v>
       </c>
       <c r="B92" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D92" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F92" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>73</v>
@@ -5395,13 +5371,13 @@
         <v>23</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D93" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>70</v>
@@ -5418,13 +5394,13 @@
         <v>23</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F94" s="21" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>69</v>
@@ -5435,13 +5411,13 @@
         <v>23</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>69</v>
@@ -5452,19 +5428,19 @@
         <v>23</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H96" s="22" t="s">
-        <v>103</v>
+      <c r="H96" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="I96" s="5" t="s">
         <v>66</v>
@@ -5475,10 +5451,10 @@
         <v>23</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D97" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>69</v>
@@ -5490,13 +5466,13 @@
         <v>23</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>69</v>
@@ -5507,13 +5483,13 @@
         <v>23</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>73</v>
@@ -5524,13 +5500,13 @@
         <v>23</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F100" s="21" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>69</v>
@@ -5541,13 +5517,13 @@
         <v>23</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D101" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>73</v>
@@ -5558,10 +5534,10 @@
         <v>23</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F102" s="21" t="s">
         <v>52</v>
@@ -5575,10 +5551,10 @@
         <v>23</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D103" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F103" s="21" t="s">
         <v>52</v>
@@ -5592,10 +5568,10 @@
         <v>23</v>
       </c>
       <c r="B104" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D104" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F104" s="21" t="s">
         <v>52</v>
@@ -5615,13 +5591,13 @@
         <v>23</v>
       </c>
       <c r="B105" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>69</v>
@@ -5632,13 +5608,13 @@
         <v>23</v>
       </c>
       <c r="B106" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>73</v>
@@ -5649,13 +5625,13 @@
         <v>23</v>
       </c>
       <c r="B107" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>69</v>
@@ -5666,13 +5642,13 @@
         <v>23</v>
       </c>
       <c r="B108" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>73</v>
@@ -5683,13 +5659,13 @@
         <v>23</v>
       </c>
       <c r="B109" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D109" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F109" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>70</v>
@@ -5706,13 +5682,13 @@
         <v>23</v>
       </c>
       <c r="B110" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D110" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F110" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>74</v>
@@ -5729,13 +5705,13 @@
         <v>23</v>
       </c>
       <c r="B111" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F111" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>69</v>
@@ -5746,13 +5722,13 @@
         <v>23</v>
       </c>
       <c r="B112" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F112" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>73</v>
@@ -5763,13 +5739,13 @@
         <v>23</v>
       </c>
       <c r="B113" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D113" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F113" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>73</v>
@@ -5780,13 +5756,13 @@
         <v>23</v>
       </c>
       <c r="B114" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D114" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F114" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>70</v>
@@ -5803,13 +5779,13 @@
         <v>23</v>
       </c>
       <c r="B115" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D115" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F115" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>69</v>
@@ -5820,13 +5796,13 @@
         <v>23</v>
       </c>
       <c r="B116" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D116" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>73</v>
@@ -5837,13 +5813,13 @@
         <v>23</v>
       </c>
       <c r="B117" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F117" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>69</v>
@@ -5854,13 +5830,13 @@
         <v>23</v>
       </c>
       <c r="B118" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F118" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>73</v>
@@ -5871,13 +5847,13 @@
         <v>23</v>
       </c>
       <c r="B119" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D119" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F119" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>70</v>
@@ -5894,19 +5870,19 @@
         <v>23</v>
       </c>
       <c r="B120" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F120" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H120" s="22" t="s">
-        <v>116</v>
+      <c r="H120" s="14" t="s">
+        <v>58</v>
       </c>
       <c r="I120" s="5" t="s">
         <v>66</v>
@@ -5917,13 +5893,13 @@
         <v>23</v>
       </c>
       <c r="B121" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F121" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>74</v>
@@ -5940,13 +5916,13 @@
         <v>23</v>
       </c>
       <c r="B122" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F122" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>69</v>
@@ -5957,13 +5933,13 @@
         <v>23</v>
       </c>
       <c r="B123" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D123" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F123" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>73</v>
@@ -5974,13 +5950,13 @@
         <v>23</v>
       </c>
       <c r="B124" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D124" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>69</v>
@@ -5991,13 +5967,13 @@
         <v>23</v>
       </c>
       <c r="B125" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D125" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F125" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>74</v>
@@ -6014,13 +5990,13 @@
         <v>23</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D126" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F126" s="21" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>69</v>
@@ -6031,32 +6007,32 @@
         <v>23</v>
       </c>
       <c r="B127" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D127" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F127" s="21"/>
     </row>
-    <row r="128" spans="1:9" ht="30">
+    <row r="128" spans="1:9" ht="28">
       <c r="A128" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B128" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D128" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F128" s="21"/>
-      <c r="H128" s="22" t="s">
-        <v>107</v>
+      <c r="H128" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="I128" s="5" t="s">
         <v>66</v>
@@ -6067,17 +6043,17 @@
         <v>23</v>
       </c>
       <c r="B129" s="24" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D129" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E129" s="3" t="s">
         <v>74</v>
       </c>
       <c r="F129" s="21"/>
       <c r="H129" s="22" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I129" s="5" t="s">
         <v>66</v>
@@ -6088,30 +6064,38 @@
         <v>23</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>67</v>
       </c>
       <c r="D130" s="20"/>
       <c r="F130" s="21"/>
-    </row>
-    <row r="131" spans="1:9" ht="70">
+      <c r="I130" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="15">
       <c r="A131" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B131" s="20" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="D131" s="20"/>
       <c r="F131" s="21"/>
+      <c r="H131" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
CS0702: Esqueleto ajustado y creación de documento de seguimiento de producción digital
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion02/EsqueletoGuion_CS_07_02_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="24360" windowHeight="14200" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="942" yWindow="0" windowWidth="24359" windowHeight="14196" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -15,11 +20,11 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -31,7 +36,7 @@
     <author>MCMarquez</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="106">
   <si>
     <t>FICHA</t>
   </si>
@@ -294,9 +299,6 @@
   </si>
   <si>
     <t>Consolidación</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: la Alta Edad Media</t>
   </si>
   <si>
     <t>Los monasterios y las órdenes religiosas</t>
@@ -2423,7 +2425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2437,13 +2439,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="22.46484375" customWidth="1"/>
     <col min="2" max="2" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15">
+    <row r="1" spans="1:2" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -2451,7 +2453,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -2459,15 +2461,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -2475,7 +2477,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -2483,7 +2485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -2506,25 +2508,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -2544,7 +2546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2564,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2604,7 +2606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2624,7 +2626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2644,7 +2646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2665,7 +2667,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2688,7 @@
       </c>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2707,7 +2709,7 @@
       </c>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2747,7 +2749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2767,7 +2769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2787,7 +2789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2807,7 +2809,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2827,7 +2829,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2847,7 +2849,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2867,7 +2869,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -2887,7 +2889,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -2907,7 +2909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2927,7 +2929,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2947,7 +2949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2967,7 +2969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2987,7 +2989,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -3007,7 +3009,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -3027,7 +3029,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -3047,7 +3049,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3067,7 +3069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -3087,7 +3089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -3107,7 +3109,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -3127,7 +3129,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -3147,7 +3149,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -3187,7 +3189,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -3207,7 +3209,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -3218,7 +3220,7 @@
         <v>51</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
         <v>53</v>
@@ -3246,14 +3248,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.46484375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -3275,7 +3277,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="15">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
         <v>62</v>
       </c>
@@ -3286,12 +3288,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -3311,24 +3313,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.46484375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -3339,7 +3341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3350,7 +3352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3361,7 +3363,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3372,7 +3374,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3383,7 +3385,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3394,7 +3396,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3416,7 +3418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3427,7 +3429,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="4" customFormat="1">
+    <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3438,7 +3440,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3449,7 +3451,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3460,7 +3462,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3471,7 +3473,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3482,7 +3484,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3504,7 +3506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3515,7 +3517,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3526,7 +3528,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3537,7 +3539,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3548,7 +3550,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3559,7 +3561,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3581,7 +3583,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3592,7 +3594,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3603,7 +3605,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3614,7 +3616,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3625,7 +3627,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3636,7 +3638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3647,7 +3649,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3658,7 +3660,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3669,7 +3671,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3680,7 +3682,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3691,7 +3693,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3702,18 +3704,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3724,7 +3726,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3753,25 +3755,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H89" sqref="H89"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1328125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1328125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.796875" style="3" customWidth="1"/>
     <col min="8" max="8" width="28" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
@@ -3800,7 +3802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15">
+    <row r="2" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
@@ -3812,7 +3814,7 @@
       </c>
       <c r="D2" s="21"/>
     </row>
-    <row r="3" spans="1:9" ht="15">
+    <row r="3" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>23</v>
       </c>
@@ -3820,13 +3822,13 @@
         <v>68</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15">
+    <row r="4" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
@@ -3834,7 +3836,7 @@
         <v>68</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>70</v>
@@ -3846,7 +3848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15">
+    <row r="5" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>23</v>
       </c>
@@ -3860,7 +3862,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30">
+    <row r="6" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>23</v>
       </c>
@@ -3874,7 +3876,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30">
+    <row r="7" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -3888,7 +3890,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30">
+    <row r="8" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
@@ -3908,7 +3910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30">
+    <row r="9" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A9" s="13" t="s">
         <v>23</v>
       </c>
@@ -3928,7 +3930,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30">
+    <row r="10" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
         <v>23</v>
       </c>
@@ -3942,7 +3944,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30">
+    <row r="11" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A11" s="13" t="s">
         <v>23</v>
       </c>
@@ -3956,7 +3958,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30">
+    <row r="12" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A12" s="13" t="s">
         <v>23</v>
       </c>
@@ -3976,7 +3978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30">
+    <row r="13" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A13" s="13" t="s">
         <v>23</v>
       </c>
@@ -3990,7 +3992,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30">
+    <row r="14" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A14" s="13" t="s">
         <v>23</v>
       </c>
@@ -4010,7 +4012,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="30">
+    <row r="15" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -4024,7 +4026,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30">
+    <row r="16" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A16" s="13" t="s">
         <v>23</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30">
+    <row r="17" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A17" s="13" t="s">
         <v>23</v>
       </c>
@@ -4058,7 +4060,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15">
+    <row r="18" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A18" s="13" t="s">
         <v>23</v>
       </c>
@@ -4072,7 +4074,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15">
+    <row r="19" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A19" s="13" t="s">
         <v>23</v>
       </c>
@@ -4086,7 +4088,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15">
+    <row r="20" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
@@ -4100,7 +4102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30">
+    <row r="21" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
@@ -4120,7 +4122,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30">
+    <row r="22" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A22" s="13" t="s">
         <v>23</v>
       </c>
@@ -4140,7 +4142,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30">
+    <row r="23" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
         <v>23</v>
       </c>
@@ -4153,14 +4155,14 @@
       <c r="E23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="22" t="s">
-        <v>78</v>
+      <c r="H23" t="s">
+        <v>62</v>
       </c>
       <c r="I23" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="45">
+    <row r="24" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A24" s="13" t="s">
         <v>23</v>
       </c>
@@ -4168,13 +4170,13 @@
         <v>68</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="45">
+    <row r="25" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A25" s="13" t="s">
         <v>23</v>
       </c>
@@ -4182,16 +4184,16 @@
         <v>68</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="45">
+    <row r="26" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A26" s="13" t="s">
         <v>23</v>
       </c>
@@ -4199,16 +4201,16 @@
         <v>68</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="45">
+    <row r="27" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A27" s="13" t="s">
         <v>23</v>
       </c>
@@ -4216,10 +4218,10 @@
         <v>68</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>70</v>
@@ -4231,7 +4233,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="45">
+    <row r="28" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A28" s="13" t="s">
         <v>23</v>
       </c>
@@ -4239,16 +4241,16 @@
         <v>68</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="45">
+    <row r="29" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A29" s="13" t="s">
         <v>23</v>
       </c>
@@ -4256,16 +4258,16 @@
         <v>68</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="45">
+    <row r="30" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A30" s="13" t="s">
         <v>23</v>
       </c>
@@ -4273,16 +4275,16 @@
         <v>68</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A31" s="13" t="s">
         <v>23</v>
       </c>
@@ -4290,10 +4292,10 @@
         <v>68</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>74</v>
@@ -4305,7 +4307,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="45">
+    <row r="32" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A32" s="13" t="s">
         <v>23</v>
       </c>
@@ -4313,16 +4315,16 @@
         <v>68</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="45">
+    <row r="33" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A33" s="13" t="s">
         <v>23</v>
       </c>
@@ -4330,16 +4332,16 @@
         <v>68</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="45">
+    <row r="34" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
         <v>23</v>
       </c>
@@ -4347,16 +4349,16 @@
         <v>68</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45">
+    <row r="35" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A35" s="13" t="s">
         <v>23</v>
       </c>
@@ -4364,16 +4366,16 @@
         <v>68</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="45">
+    <row r="36" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A36" s="13" t="s">
         <v>23</v>
       </c>
@@ -4381,16 +4383,16 @@
         <v>68</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="45">
+    <row r="37" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A37" s="13" t="s">
         <v>23</v>
       </c>
@@ -4398,16 +4400,16 @@
         <v>68</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="45">
+    <row r="38" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A38" s="13" t="s">
         <v>23</v>
       </c>
@@ -4415,16 +4417,16 @@
         <v>68</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="45">
+    <row r="39" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A39" s="13" t="s">
         <v>23</v>
       </c>
@@ -4432,16 +4434,16 @@
         <v>68</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="45">
+    <row r="40" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A40" s="13" t="s">
         <v>23</v>
       </c>
@@ -4449,16 +4451,16 @@
         <v>68</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="45">
+    <row r="41" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A41" s="13" t="s">
         <v>23</v>
       </c>
@@ -4466,16 +4468,16 @@
         <v>68</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="45">
+    <row r="42" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A42" s="13" t="s">
         <v>23</v>
       </c>
@@ -4483,16 +4485,16 @@
         <v>68</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="45.25" x14ac:dyDescent="0.45">
       <c r="A43" s="13" t="s">
         <v>23</v>
       </c>
@@ -4500,10 +4502,10 @@
         <v>68</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>70</v>
@@ -4515,7 +4517,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15">
+    <row r="44" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A44" s="13" t="s">
         <v>23</v>
       </c>
@@ -4529,10 +4531,10 @@
         <v>69</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="28">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
         <v>23</v>
       </c>
@@ -4546,7 +4548,7 @@
         <v>74</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H45" s="14" t="s">
         <v>40</v>
@@ -4555,7 +4557,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="28">
+    <row r="46" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A46" s="13" t="s">
         <v>23</v>
       </c>
@@ -4569,7 +4571,7 @@
         <v>74</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H46" s="14" t="s">
         <v>41</v>
@@ -4578,101 +4580,101 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15">
+    <row r="47" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A47" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15">
+    <row r="48" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B48" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D48" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F48" s="21"/>
     </row>
-    <row r="49" spans="1:9" ht="15">
+    <row r="49" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B49" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F49" s="21"/>
     </row>
-    <row r="50" spans="1:9" ht="15">
+    <row r="50" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A50" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B50" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F50" s="21"/>
     </row>
-    <row r="51" spans="1:9" ht="15">
+    <row r="51" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A51" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B51" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F51" s="21"/>
     </row>
-    <row r="52" spans="1:9" ht="15">
+    <row r="52" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A52" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B52" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F52" s="21"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A53" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D53" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>70</v>
@@ -4685,15 +4687,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30">
+    <row r="54" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A54" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B54" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D54" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="D54" s="21" t="s">
-        <v>81</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>74</v>
@@ -4706,75 +4708,75 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30">
+    <row r="55" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A55" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D55" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F55" s="21"/>
     </row>
-    <row r="56" spans="1:9" ht="30">
+    <row r="56" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A56" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D56" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F56" s="21"/>
     </row>
-    <row r="57" spans="1:9" ht="30">
+    <row r="57" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A57" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D57" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F57" s="21"/>
     </row>
-    <row r="58" spans="1:9" ht="30">
+    <row r="58" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A58" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>73</v>
       </c>
       <c r="F58" s="21"/>
     </row>
-    <row r="59" spans="1:9" ht="30">
+    <row r="59" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A59" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>70</v>
@@ -4787,101 +4789,101 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15">
+    <row r="60" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A60" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F60" s="21"/>
     </row>
-    <row r="61" spans="1:9" ht="60">
+    <row r="61" spans="1:9" ht="60.7" x14ac:dyDescent="0.45">
       <c r="A61" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D61" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F61" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="G61" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="60">
+    <row r="62" spans="1:9" ht="60.7" x14ac:dyDescent="0.45">
       <c r="A62" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D62" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="60">
+    <row r="63" spans="1:9" ht="60.7" x14ac:dyDescent="0.45">
       <c r="A63" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D63" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F63" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="F63" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="G63" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="60">
+    <row r="64" spans="1:9" ht="60.7" x14ac:dyDescent="0.45">
       <c r="A64" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D64" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F64" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="F64" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="G64" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="60">
+    <row r="65" spans="1:9" ht="60.7" x14ac:dyDescent="0.45">
       <c r="A65" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F65" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="F65" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>74</v>
@@ -4893,137 +4895,137 @@
         <v>66</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A66" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A67" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G67" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A68" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="30">
+    <row r="69" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A69" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30">
+    <row r="70" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A70" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G70" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30">
+    <row r="71" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A71" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G71" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="30">
+    <row r="72" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A72" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B72" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="30">
+    <row r="73" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A73" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G73" s="3" t="s">
         <v>70</v>
@@ -5035,18 +5037,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="30">
+    <row r="74" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A74" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G74" s="3" t="s">
         <v>74</v>
@@ -5058,152 +5060,152 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="15">
+    <row r="75" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A75" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F75" s="21"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A76" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B76" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D76" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F76" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="F76" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="30">
+    <row r="77" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A77" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B77" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D77" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="F77" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="G77" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="30">
+    <row r="78" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A78" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B78" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="F78" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="30">
+    <row r="79" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A79" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B79" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D79" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F79" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="F79" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="30">
+    <row r="80" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A80" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B80" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D80" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F80" s="21" t="s">
+      <c r="G80" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G80" s="3" t="s">
+    </row>
+    <row r="81" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
+      <c r="A81" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F81" s="21" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="30">
-      <c r="A81" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B81" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="D81" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F81" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="30">
+    <row r="82" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A82" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B82" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="30">
+    <row r="83" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A83" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>70</v>
@@ -5215,63 +5217,63 @@
         <v>66</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A84" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="30">
+    <row r="85" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A85" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F85" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G85" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A86" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15">
+    <row r="87" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A87" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D87" s="21" t="s">
         <v>76</v>
@@ -5281,12 +5283,12 @@
       </c>
       <c r="F87" s="21"/>
     </row>
-    <row r="88" spans="1:9" ht="15">
+    <row r="88" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A88" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D88" s="21" t="s">
         <v>76</v>
@@ -5296,12 +5298,12 @@
       </c>
       <c r="F88" s="21"/>
     </row>
-    <row r="89" spans="1:9" ht="15">
+    <row r="89" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A89" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D89" s="21" t="s">
         <v>76</v>
@@ -5317,67 +5319,67 @@
         <v>66</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A90" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D90" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F90" s="21"/>
     </row>
-    <row r="91" spans="1:9" ht="45">
+    <row r="91" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A91" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B91" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D91" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F91" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="F91" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="45">
+    <row r="92" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A92" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B92" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D92" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F92" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="G92" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="45">
+    <row r="93" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A93" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D93" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F93" s="21" t="s">
         <v>94</v>
-      </c>
-      <c r="F93" s="21" t="s">
-        <v>95</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>70</v>
@@ -5389,52 +5391,52 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A94" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D94" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F94" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G94" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="30">
+    <row r="95" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A95" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D95" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="30">
+    <row r="96" spans="1:9" ht="30.55" x14ac:dyDescent="0.45">
       <c r="A96" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D96" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G96" s="3" t="s">
         <v>74</v>
@@ -5446,98 +5448,98 @@
         <v>66</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="45">
+    <row r="97" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A97" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D97" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F97" s="21"/>
     </row>
-    <row r="98" spans="1:9" ht="45">
+    <row r="98" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A98" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D98" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G98" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="45">
+    <row r="99" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A99" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D99" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="45">
+    <row r="100" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A100" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D100" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F100" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G100" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="45">
+    <row r="101" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A101" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B101" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D101" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G101" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="45">
+    <row r="102" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A102" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D102" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F102" s="21" t="s">
         <v>52</v>
@@ -5546,15 +5548,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="45">
+    <row r="103" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A103" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D103" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F103" s="21" t="s">
         <v>52</v>
@@ -5563,15 +5565,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="45">
+    <row r="104" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A104" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B104" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D104" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F104" s="21" t="s">
         <v>52</v>
@@ -5586,86 +5588,86 @@
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="45">
+    <row r="105" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A105" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B105" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D105" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="45">
+    <row r="106" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A106" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B106" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D106" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="45">
+    <row r="107" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A107" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B107" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D107" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="45">
+    <row r="108" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A108" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B108" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D108" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="45">
+    <row r="109" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A109" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B109" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D109" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F109" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G109" s="3" t="s">
         <v>70</v>
@@ -5677,18 +5679,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="45">
+    <row r="110" spans="1:9" ht="46.4" x14ac:dyDescent="0.45">
       <c r="A110" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B110" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D110" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F110" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>74</v>
@@ -5700,69 +5702,69 @@
         <v>66</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="45">
+    <row r="111" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A111" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B111" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D111" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F111" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G111" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="45">
+    <row r="112" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A112" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B112" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D112" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F112" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G112" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="45">
+    <row r="113" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A113" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B113" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D113" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F113" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="45">
+    <row r="114" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A114" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B114" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D114" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F114" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G114" s="3" t="s">
         <v>70</v>
@@ -5774,86 +5776,86 @@
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="45">
+    <row r="115" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A115" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B115" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D115" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F115" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="45">
+    <row r="116" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A116" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B116" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D116" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="45">
+    <row r="117" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A117" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B117" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D117" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F117" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="45">
+    <row r="118" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A118" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B118" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D118" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F118" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="45">
+    <row r="119" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A119" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B119" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D119" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F119" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G119" s="3" t="s">
         <v>70</v>
@@ -5865,18 +5867,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="45">
+    <row r="120" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A120" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B120" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D120" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F120" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>70</v>
@@ -5888,18 +5890,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="45">
+    <row r="121" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A121" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B121" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D121" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F121" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>74</v>
@@ -5911,69 +5913,69 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="45">
+    <row r="122" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A122" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B122" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D122" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F122" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G122" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="45">
+    <row r="123" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A123" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B123" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D123" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F123" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="45">
+    <row r="124" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A124" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B124" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D124" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="45">
+    <row r="125" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A125" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B125" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D125" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F125" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G125" s="3" t="s">
         <v>74</v>
@@ -5985,29 +5987,29 @@
         <v>66</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="45">
+    <row r="126" spans="1:9" ht="45.65" x14ac:dyDescent="0.45">
       <c r="A126" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D126" s="21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F126" s="21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G126" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="15">
+    <row r="127" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A127" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B127" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D127" s="20" t="s">
         <v>77</v>
@@ -6017,12 +6019,12 @@
       </c>
       <c r="F127" s="21"/>
     </row>
-    <row r="128" spans="1:9" ht="28">
+    <row r="128" spans="1:9" ht="28.65" x14ac:dyDescent="0.45">
       <c r="A128" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B128" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D128" s="20" t="s">
         <v>77</v>
@@ -6038,12 +6040,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="30">
+    <row r="129" spans="1:9" ht="30.95" x14ac:dyDescent="0.45">
       <c r="A129" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B129" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D129" s="20" t="s">
         <v>77</v>
@@ -6053,18 +6055,18 @@
       </c>
       <c r="F129" s="21"/>
       <c r="H129" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I129" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="1:9" ht="15">
+    <row r="130" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A130" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B130" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>67</v>
@@ -6075,12 +6077,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="15">
+    <row r="131" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A131" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B131" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>62</v>

</xml_diff>